<commit_message>
added total profir, total volume and one point increase to pivots
</commit_message>
<xml_diff>
--- a/processed_vol_trend_data/pivots.xlsx
+++ b/processed_vol_trend_data/pivots.xlsx
@@ -417,19 +417,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
-    <col width="26" customWidth="1" min="4" max="4"/>
-    <col width="33" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="26" customWidth="1" min="6" max="6"/>
+    <col width="33" customWidth="1" min="7" max="7"/>
+    <col width="27" customWidth="1" min="8" max="8"/>
+    <col width="42" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -452,12 +456,32 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>total_profit</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>total_volume</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>typical_spread_in_points</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>weighted_avg_execution_spread_$</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>percentage_of_occurrences</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>one_point_increase_of_weighted_spread_lr</t>
         </is>
       </c>
     </row>
@@ -481,10 +505,22 @@
         <v>-8.288711069913706</v>
       </c>
       <c r="D4" t="n">
+        <v>-34979435.88</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4047717.57</v>
+      </c>
+      <c r="F4" t="n">
         <v>9.145454545452539</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
         <v>8.850136861443799</v>
+      </c>
+      <c r="H4" t="n">
+        <v>35.11586452762923</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-1.479759821313245</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +536,22 @@
         <v>-21.49854362216667</v>
       </c>
       <c r="D5" t="n">
+        <v>-50969123.26</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2243046.35</v>
+      </c>
+      <c r="F5" t="n">
         <v>9.225806451613174</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G5" t="n">
         <v>8.826627322132296</v>
+      </c>
+      <c r="H5" t="n">
+        <v>19.25133689839572</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-1.659191439800495</v>
       </c>
     </row>
     <row r="6">
@@ -519,10 +567,22 @@
         <v>2.362199022230769</v>
       </c>
       <c r="D6" t="n">
+        <v>6939455.84</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2476737.09</v>
+      </c>
+      <c r="F6" t="n">
         <v>11.01724137930831</v>
       </c>
-      <c r="E6" t="n">
+      <c r="G6" t="n">
         <v>9.375202851878555</v>
+      </c>
+      <c r="H6" t="n">
+        <v>27.80748663101604</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.09125545721933777</v>
       </c>
     </row>
     <row r="7">
@@ -538,346 +598,652 @@
         <v>-5.37864698262</v>
       </c>
       <c r="D7" t="n">
+        <v>-7614650.48</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1375866.59</v>
+      </c>
+      <c r="F7" t="n">
         <v>9.899999999999974</v>
       </c>
-      <c r="E7" t="n">
+      <c r="G7" t="n">
         <v>8.457566604326196</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="H7" t="n">
+        <v>17.825311942959</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-1.876264873612548</v>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
         <is>
           <t>GBPUSD</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
+    <row r="39">
+      <c r="B39" t="inlineStr">
         <is>
           <t>count_of_occurrences</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>total_profit</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>total_volume</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
         <is>
           <t>typical_spread_in_points</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>weighted_avg_execution_spread_$</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>percentage_of_occurrences</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>one_point_increase_of_weighted_spread_lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
         <is>
           <t>Volatility_Trend</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="41">
+      <c r="A41" t="inlineStr">
         <is>
           <t>High Volatility + No Trend</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B41" t="n">
         <v>214</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C41" t="n">
         <v>-4.070678911214953</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D41" t="n">
+        <v>-12741302.841987</v>
+      </c>
+      <c r="E41" t="n">
+        <v>2599682.23</v>
+      </c>
+      <c r="F41" t="n">
         <v>10.43617021276468</v>
       </c>
-      <c r="E11" t="n">
+      <c r="G41" t="n">
         <v>12.04392561918357</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="H41" t="n">
+        <v>38.14616755793227</v>
+      </c>
+      <c r="I41" t="n">
+        <v>-0.02839638508320652</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
         <is>
           <t>High Volatility + Trend</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B42" t="n">
         <v>82</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C42" t="n">
         <v>-44.0579731097561</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D42" t="n">
+        <v>-48833532.44791</v>
+      </c>
+      <c r="E42" t="n">
+        <v>947369.55</v>
+      </c>
+      <c r="F42" t="n">
         <v>12.45454545454414</v>
       </c>
-      <c r="E12" t="n">
+      <c r="G42" t="n">
         <v>12.58185417326494</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="H42" t="n">
+        <v>14.61675579322638</v>
+      </c>
+      <c r="I42" t="n">
+        <v>-3.488446647930592</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
         <is>
           <t>Low Volatility + No Trend</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B43" t="n">
         <v>234</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C43" t="n">
         <v>-1.380881414529914</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D43" t="n">
+        <v>-3001446.303141001</v>
+      </c>
+      <c r="E43" t="n">
+        <v>2448729.54</v>
+      </c>
+      <c r="F43" t="n">
         <v>13.47222222222156</v>
       </c>
-      <c r="E13" t="n">
+      <c r="G43" t="n">
         <v>13.47261067135606</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="H43" t="n">
+        <v>41.71122994652406</v>
+      </c>
+      <c r="I43" t="n">
+        <v>-0.006549058777956531</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
         <is>
           <t>Low Volatility + Trend</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B44" t="n">
         <v>31</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C44" t="n">
         <v>-42.58803487096774</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D44" t="n">
+        <v>-17835065.53399</v>
+      </c>
+      <c r="E44" t="n">
+        <v>323749.73</v>
+      </c>
+      <c r="F44" t="n">
         <v>11</v>
       </c>
-      <c r="E14" t="n">
+      <c r="G44" t="n">
         <v>15.6018364113038</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="H44" t="n">
+        <v>5.525846702317291</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-1.016898904927557</v>
+      </c>
+    </row>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
         <is>
           <t>USDJPY</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" t="inlineStr">
+    <row r="76">
+      <c r="B76" t="inlineStr">
         <is>
           <t>count_of_occurrences</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C76" t="inlineStr">
         <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>total_profit</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>total_volume</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
         <is>
           <t>typical_spread_in_points</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="G76" t="inlineStr">
         <is>
           <t>weighted_avg_execution_spread_$</t>
         </is>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>percentage_of_occurrences</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>one_point_increase_of_weighted_spread_lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
         <is>
           <t>Volatility_Trend</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="78">
+      <c r="A78" t="inlineStr">
         <is>
           <t>High Volatility + No Trend</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B78" t="n">
         <v>181</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C78" t="n">
         <v>-13.67256108839779</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D78" t="n">
+        <v>-13317215</v>
+      </c>
+      <c r="E78" t="n">
+        <v>901024.2</v>
+      </c>
+      <c r="F78" t="n">
         <v>13.17333333333175</v>
       </c>
-      <c r="E18" t="n">
+      <c r="G78" t="n">
         <v>10.61131960572962</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="H78" t="n">
+        <v>32.26381461675579</v>
+      </c>
+      <c r="I78" t="n">
+        <v>-4.045946811637981</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
         <is>
           <t>High Volatility + Trend</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B79" t="n">
         <v>103</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C79" t="n">
         <v>-35.49163069902912</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D79" t="n">
+        <v>-22044239</v>
+      </c>
+      <c r="E79" t="n">
+        <v>635193.35</v>
+      </c>
+      <c r="F79" t="n">
         <v>12.72222222222133</v>
       </c>
-      <c r="E19" t="n">
+      <c r="G79" t="n">
         <v>9.563869937631219</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="H79" t="n">
+        <v>18.36007130124777</v>
+      </c>
+      <c r="I79" t="n">
+        <v>-2.353777940763052</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
         <is>
           <t>Low Volatility + No Trend</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B80" t="n">
         <v>188</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C80" t="n">
         <v>-2.907438643617021</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D80" t="n">
+        <v>-1269776</v>
+      </c>
+      <c r="E80" t="n">
+        <v>418436.7</v>
+      </c>
+      <c r="F80" t="n">
         <v>15.89285714285684</v>
       </c>
-      <c r="E20" t="n">
+      <c r="G80" t="n">
         <v>10.40518699754833</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="H80" t="n">
+        <v>33.51158645276293</v>
+      </c>
+      <c r="I80" t="n">
+        <v>-1.075074353199468</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
         <is>
           <t>Low Volatility + Trend</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B81" t="n">
         <v>89</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C81" t="n">
         <v>-20.26355995505618</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D81" t="n">
+        <v>-4740458</v>
+      </c>
+      <c r="E81" t="n">
+        <v>256229.87</v>
+      </c>
+      <c r="F81" t="n">
         <v>11.93333333332963</v>
       </c>
-      <c r="E21" t="n">
+      <c r="G81" t="n">
         <v>9.942112108275058</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
+      <c r="H81" t="n">
+        <v>15.86452762923351</v>
+      </c>
+      <c r="I81" t="n">
+        <v>-6.200267236059804</v>
+      </c>
+    </row>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
         <is>
           <t>XAUUSD</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="B23" t="inlineStr">
+    <row r="113">
+      <c r="B113" t="inlineStr">
         <is>
           <t>count_of_occurrences</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C113" t="inlineStr">
         <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>total_profit</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>total_volume</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
         <is>
           <t>typical_spread_in_points</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="G113" t="inlineStr">
         <is>
           <t>weighted_avg_execution_spread_$</t>
         </is>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>percentage_of_occurrences</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>one_point_increase_of_weighted_spread_lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
         <is>
           <t>Volatility_Trend</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="115">
+      <c r="A115" t="inlineStr">
         <is>
           <t>High Volatility + No Trend</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B115" t="n">
         <v>223</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C115" t="n">
         <v>-30.3349935470852</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D115" t="n">
+        <v>-167811765.68</v>
+      </c>
+      <c r="E115" t="n">
+        <v>4905503.47</v>
+      </c>
+      <c r="F115" t="n">
         <v>20.84745762712242</v>
       </c>
-      <c r="E25" t="n">
+      <c r="G115" t="n">
         <v>27.78015214876156</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="H115" t="n">
+        <v>40.0359066427289</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0.174580775022823</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
         <is>
           <t>High Volatility + Trend</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B116" t="n">
         <v>141</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C116" t="n">
         <v>-56.62320707801418</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D116" t="n">
+        <v>-201042079.38</v>
+      </c>
+      <c r="E116" t="n">
+        <v>3039428.76</v>
+      </c>
+      <c r="F116" t="n">
         <v>20.94736842105631</v>
       </c>
-      <c r="E26" t="n">
+      <c r="G116" t="n">
         <v>31.46887424561551</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="H116" t="n">
+        <v>25.31418312387791</v>
+      </c>
+      <c r="I116" t="n">
+        <v>-0.8735817132808531</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
         <is>
           <t>Low Volatility + No Trend</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B117" t="n">
         <v>132</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C117" t="n">
         <v>14.67839834848485</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D117" t="n">
+        <v>44661475.96</v>
+      </c>
+      <c r="E117" t="n">
+        <v>2853821.63</v>
+      </c>
+      <c r="F117" t="n">
         <v>21.87500000000284</v>
       </c>
-      <c r="E27" t="n">
+      <c r="G117" t="n">
         <v>26.55715673764307</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="H117" t="n">
+        <v>23.6983842010772</v>
+      </c>
+      <c r="I117" t="n">
+        <v>0.0995374841512332</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
         <is>
           <t>Low Volatility + Trend</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B118" t="n">
         <v>61</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C118" t="n">
         <v>-0.7356025245901638</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D118" t="n">
+        <v>2137769.51</v>
+      </c>
+      <c r="E118" t="n">
+        <v>1340254.44</v>
+      </c>
+      <c r="F118" t="n">
         <v>22.15384615384874</v>
       </c>
-      <c r="E28" t="n">
+      <c r="G118" t="n">
         <v>26.91615958414931</v>
+      </c>
+      <c r="H118" t="n">
+        <v>10.95152603231598</v>
+      </c>
+      <c r="I118" t="n">
+        <v>-1.499930589854987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pct for profit and volume in pivots
</commit_message>
<xml_diff>
--- a/processed_vol_trend_data/pivots.xlsx
+++ b/processed_vol_trend_data/pivots.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,8 +432,10 @@
     <col width="33" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="46" customWidth="1" min="9" max="9"/>
+    <col width="21" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="46" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -476,10 +478,20 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>pct_total_profit</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>pct_total_volume</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>impact_on_PnL_1$_increase_of_weighted+spread</t>
         </is>
@@ -517,9 +529,15 @@
         <v>-34979435.88</v>
       </c>
       <c r="H4" t="n">
+        <v>40.38088209480964</v>
+      </c>
+      <c r="I4" t="n">
         <v>4047717.57</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
+        <v>39.9050663410838</v>
+      </c>
+      <c r="K4" t="n">
         <v>0.1157170625588717</v>
       </c>
     </row>
@@ -548,9 +566,15 @@
         <v>-50969123.26</v>
       </c>
       <c r="H5" t="n">
+        <v>58.83966121977033</v>
+      </c>
+      <c r="I5" t="n">
         <v>2243046.35</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
+        <v>22.11342858164777</v>
+      </c>
+      <c r="K5" t="n">
         <v>0.04400794454630767</v>
       </c>
     </row>
@@ -579,9 +603,15 @@
         <v>6939455.84</v>
       </c>
       <c r="H6" t="n">
+        <v>-8.011031082333684</v>
+      </c>
+      <c r="I6" t="n">
         <v>2476737.09</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
+        <v>24.41730584623592</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.3569065279908172</v>
       </c>
     </row>
@@ -610,9 +640,15 @@
         <v>-7614650.48</v>
       </c>
       <c r="H7" t="n">
+        <v>8.790487767753721</v>
+      </c>
+      <c r="I7" t="n">
         <v>1375866.59</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
+        <v>13.5641992310325</v>
+      </c>
+      <c r="K7" t="n">
         <v>0.1806867686985417</v>
       </c>
     </row>
@@ -656,10 +692,20 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>pct_total_profit</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>pct_total_volume</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>impact_on_PnL_1$_increase_of_weighted+spread</t>
         </is>
@@ -697,9 +743,15 @@
         <v>-12741302.841987</v>
       </c>
       <c r="H11" t="n">
+        <v>15.46061711908153</v>
+      </c>
+      <c r="I11" t="n">
         <v>2599682.23</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
+        <v>41.13726492411173</v>
+      </c>
+      <c r="K11" t="n">
         <v>0.2040358244553412</v>
       </c>
     </row>
@@ -728,9 +780,15 @@
         <v>-48833532.44791</v>
       </c>
       <c r="H12" t="n">
+        <v>59.25583569534241</v>
+      </c>
+      <c r="I12" t="n">
         <v>947369.55</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
+        <v>14.99113688190518</v>
+      </c>
+      <c r="K12" t="n">
         <v>0.01939997994227726</v>
       </c>
     </row>
@@ -759,9 +817,15 @@
         <v>-3001446.303141001</v>
       </c>
       <c r="H13" t="n">
+        <v>3.642030385105345</v>
+      </c>
+      <c r="I13" t="n">
         <v>2448729.54</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
+        <v>38.74859575221171</v>
+      </c>
+      <c r="K13" t="n">
         <v>0.8158498579292973</v>
       </c>
     </row>
@@ -790,9 +854,15 @@
         <v>-17835065.53399</v>
       </c>
       <c r="H14" t="n">
+        <v>21.64151680047071</v>
+      </c>
+      <c r="I14" t="n">
         <v>323749.73</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
+        <v>5.123002441771371</v>
+      </c>
+      <c r="K14" t="n">
         <v>0.01815242727216219</v>
       </c>
     </row>
@@ -836,10 +906,20 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
+          <t>pct_total_profit</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>pct_total_volume</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>impact_on_PnL_1$_increase_of_weighted+spread</t>
         </is>
@@ -877,9 +957,15 @@
         <v>-13317215</v>
       </c>
       <c r="H18" t="n">
+        <v>32.18919904839271</v>
+      </c>
+      <c r="I18" t="n">
         <v>901024.2</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
+        <v>40.75402197017907</v>
+      </c>
+      <c r="K18" t="n">
         <v>0.06765860579708295</v>
       </c>
     </row>
@@ -908,9 +994,15 @@
         <v>-22044239</v>
       </c>
       <c r="H19" t="n">
+        <v>53.28339273949857</v>
+      </c>
+      <c r="I19" t="n">
         <v>635193.35</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
+        <v>28.73028686822357</v>
+      </c>
+      <c r="K19" t="n">
         <v>0.02881448300392678</v>
       </c>
     </row>
@@ -939,9 +1031,15 @@
         <v>-1269776</v>
       </c>
       <c r="H20" t="n">
+        <v>3.069190698721309</v>
+      </c>
+      <c r="I20" t="n">
         <v>418436.7</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
+        <v>18.92621581632239</v>
+      </c>
+      <c r="K20" t="n">
         <v>0.3295358393921448</v>
       </c>
     </row>
@@ -970,9 +1068,15 @@
         <v>-4740458</v>
       </c>
       <c r="H21" t="n">
+        <v>11.45821751338742</v>
+      </c>
+      <c r="I21" t="n">
         <v>256229.87</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
+        <v>11.58947534527499</v>
+      </c>
+      <c r="K21" t="n">
         <v>0.0540517118810039</v>
       </c>
     </row>
@@ -1016,10 +1120,20 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
+          <t>pct_total_profit</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>pct_total_volume</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>impact_on_PnL_1$_increase_of_weighted+spread</t>
         </is>
@@ -1057,9 +1171,15 @@
         <v>-167811765.68</v>
       </c>
       <c r="H25" t="n">
+        <v>52.10661977616129</v>
+      </c>
+      <c r="I25" t="n">
         <v>4905503.47</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
+        <v>40.4110727068207</v>
+      </c>
+      <c r="K25" t="n">
         <v>0.02923217838822039</v>
       </c>
     </row>
@@ -1088,9 +1208,15 @@
         <v>-201042079.38</v>
       </c>
       <c r="H26" t="n">
+        <v>62.42484337622932</v>
+      </c>
+      <c r="I26" t="n">
         <v>3039428.76</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
+        <v>25.03852608783536</v>
+      </c>
+      <c r="K26" t="n">
         <v>0.01511837108615963</v>
       </c>
     </row>
@@ -1119,9 +1245,15 @@
         <v>44661475.96</v>
       </c>
       <c r="H27" t="n">
+        <v>-13.86767213287978</v>
+      </c>
+      <c r="I27" t="n">
         <v>2853821.63</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
+        <v>23.50951214029568</v>
+      </c>
+      <c r="K27" t="n">
         <v>0.06389895471784135</v>
       </c>
     </row>
@@ -1150,9 +1282,15 @@
         <v>2137769.51</v>
       </c>
       <c r="H28" t="n">
+        <v>-0.6637910195108355</v>
+      </c>
+      <c r="I28" t="n">
         <v>1340254.44</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
+        <v>11.04088906504825</v>
+      </c>
+      <c r="K28" t="n">
         <v>0.6269405722790011</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed old versions of the files
</commit_message>
<xml_diff>
--- a/processed_vol_trend_data/pivots.xlsx
+++ b/processed_vol_trend_data/pivots.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,12 +430,13 @@
     <col width="27" customWidth="1" min="3" max="3"/>
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="33" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="35" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="21" customWidth="1" min="10" max="10"/>
-    <col width="31" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="31" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,30 +469,35 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>volume_weighted_avg_spread_in_USD</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>total_profit</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>pct_total_profit</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>pct_total_volume</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -523,21 +529,24 @@
         <v>11.52873841586667</v>
       </c>
       <c r="F4" t="n">
+        <v>11.2826327013138</v>
+      </c>
+      <c r="G4" t="n">
         <v>-22.31079298290218</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>-7385434.04</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>79.93732156645018</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>331025.17</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>27.49571529303465</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0.04482135622729087</v>
       </c>
     </row>
@@ -560,21 +569,24 @@
         <v>10.06054773733333</v>
       </c>
       <c r="F5" t="n">
+        <v>10.20510549211238</v>
+      </c>
+      <c r="G5" t="n">
         <v>-37.16917871734376</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>-3243458.36</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>35.10604420897531</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>87262.03999999999</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>7.248186618949252</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0.0269040111863807</v>
       </c>
     </row>
@@ -597,21 +609,24 @@
         <v>13.207135400325</v>
       </c>
       <c r="F6" t="n">
+        <v>11.42664613780947</v>
+      </c>
+      <c r="G6" t="n">
         <v>1.596504929547001</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>960293.6599999999</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>-10.39387836678091</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>601497.46</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>49.96176849525823</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0.6263682507286366</v>
       </c>
     </row>
@@ -634,21 +649,24 @@
         <v>8.28290106275</v>
       </c>
       <c r="F7" t="n">
+        <v>8.282943930626022</v>
+      </c>
+      <c r="G7" t="n">
         <v>2.332948045628433</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>429567.59</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>-4.649487408644574</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>184130.8</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>15.29432959275787</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0.4286422073881319</v>
       </c>
     </row>
@@ -682,30 +700,35 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>volume_weighted_avg_spread_in_USD</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>total_profit</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>pct_total_profit</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>pct_total_volume</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -737,21 +760,24 @@
         <v>15.02577777517241</v>
       </c>
       <c r="F11" t="n">
+        <v>14.83735353158003</v>
+      </c>
+      <c r="G11" t="n">
         <v>-1.914570595259051</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>-803660.6699999998</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>-51.76614222686794</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>419760.27</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>45.84638776602119</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0.5223103303039579</v>
       </c>
     </row>
@@ -774,21 +800,24 @@
         <v>15.76335100813513</v>
       </c>
       <c r="F12" t="n">
+        <v>14.39382169432019</v>
+      </c>
+      <c r="G12" t="n">
         <v>4.752019024280488</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>2356143.88669</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>151.7661422268679</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>495819.54</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>54.15361223397881</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>0.2104368679692759</v>
       </c>
     </row>
@@ -822,30 +851,35 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t>volume_weighted_avg_spread_in_USD</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>total_profit</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>pct_total_profit</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>pct_total_volume</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -877,21 +911,24 @@
         <v>11.84019373696296</v>
       </c>
       <c r="F16" t="n">
+        <v>11.9027311541665</v>
+      </c>
+      <c r="G16" t="n">
         <v>-12.55590737598241</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>-2458573.73</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>69.0336336995824</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>195810.12</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>49.25805803074147</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0.0796437859929464</v>
       </c>
     </row>
@@ -914,21 +951,24 @@
         <v>13.71675476181818</v>
       </c>
       <c r="F17" t="n">
+        <v>13.77828987307455</v>
+      </c>
+      <c r="G17" t="n">
         <v>-6.866773489813938</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>-426187.67</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>11.96680951197608</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>62065.2</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>15.61314207503461</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0.1456288024475227</v>
       </c>
     </row>
@@ -951,21 +991,24 @@
         <v>12.16033729576923</v>
       </c>
       <c r="F18" t="n">
+        <v>11.54599846330231</v>
+      </c>
+      <c r="G18" t="n">
         <v>-1.749882918421034</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>-243505.15</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>6.837315929940352</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>139155.11</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>35.0059051271416</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>0.5714668047061837</v>
       </c>
     </row>
@@ -988,21 +1031,24 @@
         <v>52.46284009</v>
       </c>
       <c r="F19" t="n">
+        <v>60.70948392535197</v>
+      </c>
+      <c r="G19" t="n">
         <v>-886.6349865924304</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>-433147.79</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>12.16224085850118</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>488.53</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>0.1228947670823047</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>0.001127859846635717</v>
       </c>
     </row>
@@ -1036,30 +1082,35 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>volume_weighted_avg_spread_in_USD</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>total_profit</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>pct_total_profit</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>pct_total_volume</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -1091,21 +1142,24 @@
         <v>28.71456903</v>
       </c>
       <c r="F23" t="n">
+        <v>28.2763339998281</v>
+      </c>
+      <c r="G23" t="n">
         <v>-60.88178523553964</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>-13451782.96</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>24.61340334378907</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>220949.22</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>13.29859151559024</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>0.01642527393260886</v>
       </c>
     </row>
@@ -1128,21 +1182,24 @@
         <v>27.6892510108</v>
       </c>
       <c r="F24" t="n">
+        <v>27.71893333892316</v>
+      </c>
+      <c r="G24" t="n">
         <v>-68.34376297426078</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>-44970848.72</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>82.28542205515042</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>658009.55</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>39.60457619541428</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>0.01463191308878638</v>
       </c>
     </row>
@@ -1165,21 +1222,24 @@
         <v>25.25099210428571</v>
       </c>
       <c r="F25" t="n">
+        <v>25.30695057091755</v>
+      </c>
+      <c r="G25" t="n">
         <v>-3.064873985655785</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>-1150263.42</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>2.10469478969844</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>375305.29</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>22.58904442093136</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>0.3262776886358778</v>
       </c>
     </row>
@@ -1202,21 +1262,24 @@
         <v>27.0148432</v>
       </c>
       <c r="F26" t="n">
+        <v>27.17329847727988</v>
+      </c>
+      <c r="G26" t="n">
         <v>12.08452505846125</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>4920627.91</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>-9.003520188637943</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>407184.22</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>24.50778786806412</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>0.08275045938192063</v>
       </c>
     </row>

</xml_diff>